<commit_message>
se realiaron modificaciones en la busqueda para identificar la totalidad de los elementos tras realizar busquedas
</commit_message>
<xml_diff>
--- a/data/ChedrahuiQA_Lexico.xlsx
+++ b/data/ChedrahuiQA_Lexico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\atcon\Desktop\Playwright\playwright-piloto2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2B1E94-FDA6-4F34-A429-C182076168CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{471E1BE7-EA53-4D2E-9F24-C536442A7335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resto" sheetId="8" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Bajo CTR'!$A$1:$P$102</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Errores Ortográficos'!$A$1:$B$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Frecuencia Alta'!$A$1:$A$10</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Long Tail'!$A$1:$A$10</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Long Tail'!$A$1:$A$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Resultados Vacíos'!$A$1:$M$102</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Semánticos!$B$1:$O$1</definedName>
   </definedNames>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="585">
   <si>
     <t>QA que ejecuta</t>
   </si>
@@ -1303,33 +1303,6 @@
     <t>Caldo de pollo para sopa</t>
   </si>
   <si>
-    <t>shampoo para cabello teñido sin sulfatos</t>
-  </si>
-  <si>
-    <t>papel higiénico de 16 rollos triple hoja</t>
-  </si>
-  <si>
-    <t>café soluble descafeinado frasco grande</t>
-  </si>
-  <si>
-    <t>leche deslactosada light de un litro</t>
-  </si>
-  <si>
-    <t>refrigerador de dos puertas con despachador de hielo</t>
-  </si>
-  <si>
-    <t>desodorante en aerosol para hombre sin alcohol</t>
-  </si>
-  <si>
-    <t>pañales para bebé etapa 4 caja con 120</t>
-  </si>
-  <si>
-    <t>lavadora automática de 20 kg con carga frontal</t>
-  </si>
-  <si>
-    <t>yogurt griego sin azúcar sabor natural</t>
-  </si>
-  <si>
     <t>aceite de canola para freír 3 litros</t>
   </si>
   <si>
@@ -1826,6 +1799,12 @@
   </si>
   <si>
     <t>pañales, pañal, Pampers, KleenBebé</t>
+  </si>
+  <si>
+    <t>impresoras</t>
+  </si>
+  <si>
+    <t>samsung</t>
   </si>
 </sst>
 </file>
@@ -1983,7 +1962,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2039,6 +2018,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2383,7 +2363,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>586</v>
+        <v>577</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -2394,7 +2374,7 @@
         <v>350</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>518</v>
+        <v>509</v>
       </c>
       <c r="D2" s="25">
         <v>5</v>
@@ -2439,7 +2419,7 @@
         <v>351</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>519</v>
+        <v>510</v>
       </c>
       <c r="D3" s="25">
         <v>0</v>
@@ -2484,7 +2464,7 @@
         <v>352</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>520</v>
+        <v>511</v>
       </c>
       <c r="D4" s="25">
         <v>2</v>
@@ -2529,7 +2509,7 @@
         <v>353</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>521</v>
+        <v>512</v>
       </c>
       <c r="D5" s="25">
         <v>4</v>
@@ -2574,7 +2554,7 @@
         <v>354</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>522</v>
+        <v>513</v>
       </c>
       <c r="D6" s="25">
         <v>1</v>
@@ -2619,7 +2599,7 @@
         <v>355</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>523</v>
+        <v>514</v>
       </c>
       <c r="D7" s="25">
         <v>0</v>
@@ -2664,7 +2644,7 @@
         <v>356</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>524</v>
+        <v>515</v>
       </c>
       <c r="D8" s="25">
         <v>1</v>
@@ -2708,7 +2688,7 @@
         <v>357</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>525</v>
+        <v>516</v>
       </c>
       <c r="D9" s="25">
         <v>5</v>
@@ -2753,7 +2733,7 @@
         <v>358</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>526</v>
+        <v>517</v>
       </c>
       <c r="D10" s="25">
         <v>0</v>
@@ -2798,7 +2778,7 @@
         <v>359</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
       <c r="D11" s="25">
         <v>0</v>
@@ -2843,7 +2823,7 @@
         <v>360</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>528</v>
+        <v>519</v>
       </c>
       <c r="D12" s="25">
         <v>0</v>
@@ -2888,7 +2868,7 @@
         <v>361</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>529</v>
+        <v>520</v>
       </c>
       <c r="D13" s="25">
         <v>0</v>
@@ -2933,7 +2913,7 @@
         <v>362</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>530</v>
+        <v>521</v>
       </c>
       <c r="D14" s="25">
         <v>0</v>
@@ -2978,7 +2958,7 @@
         <v>363</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>531</v>
+        <v>522</v>
       </c>
       <c r="D15" s="25">
         <v>5</v>
@@ -3023,7 +3003,7 @@
         <v>364</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>532</v>
+        <v>523</v>
       </c>
       <c r="D16" s="25">
         <v>1</v>
@@ -3068,7 +3048,7 @@
         <v>365</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>533</v>
+        <v>524</v>
       </c>
       <c r="D17" s="25">
         <v>5</v>
@@ -3113,7 +3093,7 @@
         <v>366</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
       <c r="D18" s="25">
         <v>5</v>
@@ -3158,7 +3138,7 @@
         <v>367</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>535</v>
+        <v>526</v>
       </c>
       <c r="D19" s="25">
         <v>5</v>
@@ -3203,7 +3183,7 @@
         <v>368</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>536</v>
+        <v>527</v>
       </c>
       <c r="D20" s="25">
         <v>3</v>
@@ -3248,7 +3228,7 @@
         <v>369</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>537</v>
+        <v>528</v>
       </c>
       <c r="D21" s="25">
         <v>5</v>
@@ -3293,7 +3273,7 @@
         <v>370</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>538</v>
+        <v>529</v>
       </c>
       <c r="D22" s="25">
         <v>1</v>
@@ -3338,7 +3318,7 @@
         <v>371</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>539</v>
+        <v>530</v>
       </c>
       <c r="D23" s="25">
         <v>0</v>
@@ -3383,7 +3363,7 @@
         <v>372</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>540</v>
+        <v>531</v>
       </c>
       <c r="D24" s="25">
         <v>5</v>
@@ -3428,7 +3408,7 @@
         <v>373</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>541</v>
+        <v>532</v>
       </c>
       <c r="D25" s="25">
         <v>2</v>
@@ -3473,7 +3453,7 @@
         <v>374</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>542</v>
+        <v>533</v>
       </c>
       <c r="D26" s="25">
         <v>0</v>
@@ -3518,7 +3498,7 @@
         <v>375</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>543</v>
+        <v>534</v>
       </c>
       <c r="D27" s="25">
         <v>1</v>
@@ -3563,7 +3543,7 @@
         <v>376</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>544</v>
+        <v>535</v>
       </c>
       <c r="D28" s="25">
         <v>5</v>
@@ -3608,7 +3588,7 @@
         <v>377</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>545</v>
+        <v>536</v>
       </c>
       <c r="D29" s="25">
         <v>3</v>
@@ -3653,7 +3633,7 @@
         <v>378</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>546</v>
+        <v>537</v>
       </c>
       <c r="D30" s="25">
         <v>4</v>
@@ -3698,7 +3678,7 @@
         <v>379</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>547</v>
+        <v>538</v>
       </c>
       <c r="D31" s="25">
         <v>5</v>
@@ -3743,7 +3723,7 @@
         <v>380</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>548</v>
+        <v>539</v>
       </c>
       <c r="D32" s="25">
         <v>3</v>
@@ -3788,7 +3768,7 @@
         <v>381</v>
       </c>
       <c r="C33" s="28" t="s">
-        <v>549</v>
+        <v>540</v>
       </c>
       <c r="D33" s="28">
         <v>0</v>
@@ -3833,7 +3813,7 @@
         <v>382</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>550</v>
+        <v>541</v>
       </c>
       <c r="D34" s="25">
         <v>1</v>
@@ -3878,7 +3858,7 @@
         <v>383</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>551</v>
+        <v>542</v>
       </c>
       <c r="D35" s="25">
         <v>5</v>
@@ -3923,7 +3903,7 @@
         <v>384</v>
       </c>
       <c r="C36" s="21" t="s">
-        <v>584</v>
+        <v>575</v>
       </c>
       <c r="D36" s="21">
         <v>5</v>
@@ -3968,7 +3948,7 @@
         <v>385</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>552</v>
+        <v>543</v>
       </c>
       <c r="D37" s="21">
         <v>5</v>
@@ -4013,7 +3993,7 @@
         <v>386</v>
       </c>
       <c r="C38" s="21" t="s">
-        <v>553</v>
+        <v>544</v>
       </c>
       <c r="D38" s="21">
         <v>0</v>
@@ -4058,7 +4038,7 @@
         <v>387</v>
       </c>
       <c r="C39" s="21" t="s">
-        <v>554</v>
+        <v>545</v>
       </c>
       <c r="D39" s="21">
         <v>5</v>
@@ -4103,7 +4083,7 @@
         <v>388</v>
       </c>
       <c r="C40" s="21" t="s">
-        <v>555</v>
+        <v>546</v>
       </c>
       <c r="D40" s="21">
         <v>0</v>
@@ -4148,7 +4128,7 @@
         <v>389</v>
       </c>
       <c r="C41" s="21" t="s">
-        <v>556</v>
+        <v>547</v>
       </c>
       <c r="D41" s="21">
         <v>4</v>
@@ -4193,7 +4173,7 @@
         <v>390</v>
       </c>
       <c r="C42" s="21" t="s">
-        <v>557</v>
+        <v>548</v>
       </c>
       <c r="D42" s="21">
         <v>5</v>
@@ -4238,7 +4218,7 @@
         <v>391</v>
       </c>
       <c r="C43" s="21" t="s">
-        <v>558</v>
+        <v>549</v>
       </c>
       <c r="D43" s="21">
         <v>0</v>
@@ -4283,7 +4263,7 @@
         <v>392</v>
       </c>
       <c r="C44" s="21" t="s">
-        <v>559</v>
+        <v>550</v>
       </c>
       <c r="D44" s="21">
         <v>5</v>
@@ -4328,7 +4308,7 @@
         <v>393</v>
       </c>
       <c r="C45" s="21" t="s">
-        <v>560</v>
+        <v>551</v>
       </c>
       <c r="D45" s="21">
         <v>5</v>
@@ -4373,7 +4353,7 @@
         <v>394</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>561</v>
+        <v>552</v>
       </c>
       <c r="D46" s="21">
         <v>4</v>
@@ -4418,7 +4398,7 @@
         <v>395</v>
       </c>
       <c r="C47" s="21" t="s">
-        <v>562</v>
+        <v>553</v>
       </c>
       <c r="D47" s="21">
         <v>2</v>
@@ -4463,7 +4443,7 @@
         <v>396</v>
       </c>
       <c r="C48" s="21" t="s">
-        <v>563</v>
+        <v>554</v>
       </c>
       <c r="D48" s="21">
         <v>5</v>
@@ -4508,7 +4488,7 @@
         <v>397</v>
       </c>
       <c r="C49" s="21" t="s">
-        <v>564</v>
+        <v>555</v>
       </c>
       <c r="D49" s="21">
         <v>0</v>
@@ -4553,7 +4533,7 @@
         <v>398</v>
       </c>
       <c r="C50" s="21" t="s">
-        <v>565</v>
+        <v>556</v>
       </c>
       <c r="D50" s="21">
         <v>0</v>
@@ -4598,7 +4578,7 @@
         <v>399</v>
       </c>
       <c r="C51" s="21" t="s">
-        <v>566</v>
+        <v>557</v>
       </c>
       <c r="D51" s="21">
         <v>0</v>
@@ -4643,7 +4623,7 @@
         <v>400</v>
       </c>
       <c r="C52" s="21" t="s">
-        <v>567</v>
+        <v>558</v>
       </c>
       <c r="D52" s="21">
         <v>0</v>
@@ -4688,7 +4668,7 @@
         <v>401</v>
       </c>
       <c r="C53" s="21" t="s">
-        <v>568</v>
+        <v>559</v>
       </c>
       <c r="D53" s="21">
         <v>0</v>
@@ -4733,7 +4713,7 @@
         <v>402</v>
       </c>
       <c r="C54" s="21" t="s">
-        <v>569</v>
+        <v>560</v>
       </c>
       <c r="D54" s="21">
         <v>5</v>
@@ -4778,7 +4758,7 @@
         <v>403</v>
       </c>
       <c r="C55" s="21" t="s">
-        <v>570</v>
+        <v>561</v>
       </c>
       <c r="D55" s="21">
         <v>5</v>
@@ -4823,7 +4803,7 @@
         <v>404</v>
       </c>
       <c r="C56" s="21" t="s">
-        <v>571</v>
+        <v>562</v>
       </c>
       <c r="D56" s="21">
         <v>1</v>
@@ -4868,7 +4848,7 @@
         <v>405</v>
       </c>
       <c r="C57" s="21" t="s">
-        <v>572</v>
+        <v>563</v>
       </c>
       <c r="D57" s="21">
         <v>5</v>
@@ -4913,7 +4893,7 @@
         <v>406</v>
       </c>
       <c r="C58" s="21" t="s">
-        <v>573</v>
+        <v>564</v>
       </c>
       <c r="D58" s="21">
         <v>5</v>
@@ -4958,7 +4938,7 @@
         <v>407</v>
       </c>
       <c r="C59" s="21" t="s">
-        <v>574</v>
+        <v>565</v>
       </c>
       <c r="D59" s="21">
         <v>0</v>
@@ -5003,7 +4983,7 @@
         <v>408</v>
       </c>
       <c r="C60" s="21" t="s">
-        <v>575</v>
+        <v>566</v>
       </c>
       <c r="D60" s="21">
         <v>5</v>
@@ -5048,7 +5028,7 @@
         <v>409</v>
       </c>
       <c r="C61" s="21" t="s">
-        <v>576</v>
+        <v>567</v>
       </c>
       <c r="D61" s="21">
         <v>0</v>
@@ -5093,7 +5073,7 @@
         <v>410</v>
       </c>
       <c r="C62" s="21" t="s">
-        <v>577</v>
+        <v>568</v>
       </c>
       <c r="D62" s="21">
         <v>5</v>
@@ -5138,7 +5118,7 @@
         <v>411</v>
       </c>
       <c r="C63" s="21" t="s">
-        <v>578</v>
+        <v>569</v>
       </c>
       <c r="D63" s="21">
         <v>5</v>
@@ -5183,7 +5163,7 @@
         <v>412</v>
       </c>
       <c r="C64" s="21" t="s">
-        <v>579</v>
+        <v>570</v>
       </c>
       <c r="D64" s="21">
         <v>1</v>
@@ -5228,7 +5208,7 @@
         <v>413</v>
       </c>
       <c r="C65" s="21" t="s">
-        <v>580</v>
+        <v>571</v>
       </c>
       <c r="D65" s="21">
         <v>5</v>
@@ -5273,7 +5253,7 @@
         <v>414</v>
       </c>
       <c r="C66" s="21" t="s">
-        <v>581</v>
+        <v>572</v>
       </c>
       <c r="D66" s="21">
         <v>5</v>
@@ -5318,7 +5298,7 @@
         <v>415</v>
       </c>
       <c r="C67" s="21" t="s">
-        <v>582</v>
+        <v>573</v>
       </c>
       <c r="D67" s="21">
         <v>4</v>
@@ -5363,7 +5343,7 @@
         <v>416</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>583</v>
+        <v>574</v>
       </c>
       <c r="D68" s="22">
         <v>5</v>
@@ -5408,7 +5388,7 @@
         <v>326</v>
       </c>
       <c r="C69" s="33" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
       <c r="D69" s="33">
         <v>1</v>
@@ -5453,7 +5433,7 @@
         <v>327</v>
       </c>
       <c r="C70" s="33" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
       <c r="D70" s="33">
         <v>3</v>
@@ -5497,7 +5477,7 @@
         <v>328</v>
       </c>
       <c r="C71" s="33" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
       <c r="D71" s="33">
         <v>1</v>
@@ -5541,7 +5521,7 @@
         <v>329</v>
       </c>
       <c r="C72" s="33" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="D72" s="33">
         <v>1</v>
@@ -5585,7 +5565,7 @@
         <v>330</v>
       </c>
       <c r="C73" s="33" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
       <c r="D73" s="33">
         <v>1</v>
@@ -5629,7 +5609,7 @@
         <v>331</v>
       </c>
       <c r="C74" s="33" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
       <c r="D74" s="33">
         <v>1</v>
@@ -5674,7 +5654,7 @@
         <v>332</v>
       </c>
       <c r="C75" s="33" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
       <c r="D75" s="33">
         <v>1</v>
@@ -5718,7 +5698,7 @@
         <v>333</v>
       </c>
       <c r="C76" s="33" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
       <c r="D76" s="33">
         <v>0</v>
@@ -5763,7 +5743,7 @@
         <v>334</v>
       </c>
       <c r="C77" s="33" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
       <c r="D77" s="33">
         <v>5</v>
@@ -5807,7 +5787,7 @@
         <v>335</v>
       </c>
       <c r="C78" s="33" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
       <c r="D78" s="33">
         <v>5</v>
@@ -5851,7 +5831,7 @@
         <v>336</v>
       </c>
       <c r="C79" s="33" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
       <c r="D79" s="33">
         <v>0</v>
@@ -5896,7 +5876,7 @@
         <v>337</v>
       </c>
       <c r="C80" s="33" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
       <c r="D80" s="33">
         <v>5</v>
@@ -5940,7 +5920,7 @@
         <v>338</v>
       </c>
       <c r="C81" s="33" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
       <c r="D81" s="33">
         <v>0</v>
@@ -5985,7 +5965,7 @@
         <v>339</v>
       </c>
       <c r="C82" s="33" t="s">
-        <v>507</v>
+        <v>498</v>
       </c>
       <c r="D82" s="33">
         <v>1</v>
@@ -6029,7 +6009,7 @@
         <v>340</v>
       </c>
       <c r="C83" s="33" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
       <c r="D83" s="33">
         <v>0</v>
@@ -6074,7 +6054,7 @@
         <v>341</v>
       </c>
       <c r="C84" s="33" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
       <c r="D84" s="33">
         <v>0</v>
@@ -6119,7 +6099,7 @@
         <v>342</v>
       </c>
       <c r="C85" s="33" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
       <c r="D85" s="33">
         <v>5</v>
@@ -6163,7 +6143,7 @@
         <v>343</v>
       </c>
       <c r="C86" s="33" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
       <c r="D86" s="33">
         <v>1</v>
@@ -6208,7 +6188,7 @@
         <v>344</v>
       </c>
       <c r="C87" s="33" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
       <c r="D87" s="33">
         <v>1</v>
@@ -6253,7 +6233,7 @@
         <v>345</v>
       </c>
       <c r="C88" s="33" t="s">
-        <v>513</v>
+        <v>504</v>
       </c>
       <c r="D88" s="33">
         <v>0</v>
@@ -6298,7 +6278,7 @@
         <v>346</v>
       </c>
       <c r="C89" s="33" t="s">
-        <v>514</v>
+        <v>505</v>
       </c>
       <c r="D89" s="33">
         <v>3</v>
@@ -6342,7 +6322,7 @@
         <v>347</v>
       </c>
       <c r="C90" s="33" t="s">
-        <v>515</v>
+        <v>506</v>
       </c>
       <c r="D90" s="33">
         <v>0</v>
@@ -6387,7 +6367,7 @@
         <v>348</v>
       </c>
       <c r="C91" s="33" t="s">
-        <v>516</v>
+        <v>507</v>
       </c>
       <c r="D91" s="33">
         <v>0</v>
@@ -6432,7 +6412,7 @@
         <v>349</v>
       </c>
       <c r="C92" s="35" t="s">
-        <v>517</v>
+        <v>508</v>
       </c>
       <c r="D92" s="33">
         <v>5</v>
@@ -6470,7 +6450,7 @@
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" s="30" t="s">
-        <v>585</v>
+        <v>576</v>
       </c>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.3">
@@ -6931,103 +6911,103 @@
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185" s="38" t="s">
-        <v>587</v>
+        <v>578</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186" s="39" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187" s="39" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188" s="39" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189" s="39" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190" s="39" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191" s="39" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192" s="12" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" s="12" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="B193" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="12" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
       <c r="B194" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="12" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="B195" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="12" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
       <c r="B196" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" s="12" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="B197" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="12" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
       <c r="B198" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
     </row>
     <row r="199" spans="1:2" ht="144" x14ac:dyDescent="0.3">
       <c r="A199" s="12" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="B199" s="23" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="12" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
       <c r="B200" t="s">
         <v>54</v>
@@ -7035,7 +7015,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="12" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
       <c r="B201" t="s">
         <v>55</v>
@@ -7043,7 +7023,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="40" t="s">
-        <v>588</v>
+        <v>579</v>
       </c>
       <c r="B202" t="s">
         <v>57</v>
@@ -7051,100 +7031,100 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="B203" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
       <c r="B204" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="B205" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="B206" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
       <c r="B207" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A218" s="3" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>
@@ -16641,7 +16621,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -16685,7 +16665,7 @@
         <v>317</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>590</v>
+        <v>581</v>
       </c>
       <c r="D2" s="9">
         <v>0</v>
@@ -16730,7 +16710,7 @@
         <v>318</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
       <c r="D3" s="9">
         <v>1</v>
@@ -16774,7 +16754,7 @@
         <v>319</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="D4" s="9">
         <v>0</v>
@@ -16819,7 +16799,7 @@
         <v>320</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
       <c r="D5" s="9">
         <v>2</v>
@@ -16864,7 +16844,7 @@
         <v>321</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="D6" s="9">
         <v>1</v>
@@ -16909,7 +16889,7 @@
         <v>322</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
       <c r="D7" s="9">
         <v>1</v>
@@ -16954,7 +16934,7 @@
         <v>323</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="D8" s="9">
         <v>0</v>
@@ -16999,7 +16979,7 @@
         <v>324</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
       <c r="D9" s="9">
         <v>0</v>
@@ -17044,7 +17024,7 @@
         <v>325</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="D10" s="9">
         <v>1</v>
@@ -17159,10 +17139,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28555630-8AA8-4C83-B7EB-C61073BD67A5}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17170,60 +17150,28 @@
     <col min="1" max="1" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="12" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="12" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="12" t="s">
-        <v>423</v>
-      </c>
-      <c r="D8" s="21"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
-        <v>425</v>
-      </c>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="41" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" s="21" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="21"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A10" xr:uid="{28555630-8AA8-4C83-B7EB-C61073BD67A5}"/>
+  <autoFilter ref="A1" xr:uid="{28555630-8AA8-4C83-B7EB-C61073BD67A5}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17231,8 +17179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A479586D-24F4-4D87-B01B-4E29F29415E8}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17246,12 +17194,12 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -17259,63 +17207,63 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
       <c r="B3" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
       <c r="B4" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
       <c r="B5" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
       <c r="B6" t="s">
-        <v>591</v>
+        <v>582</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="B7" t="s">
-        <v>589</v>
+        <v>580</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="B8" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="B10" t="s">
         <v>34</v>

</xml_diff>